<commit_message>
reduced 100mm beam expansion lens diameter
</commit_message>
<xml_diff>
--- a/LifeHack-Parts.xlsx
+++ b/LifeHack-Parts.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshe\Documents\GitHub\LifeHackWebsite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\LifeHack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757EE47A-3A0F-44B2-8157-C30FD56912FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Excitation Module" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Other Hardware" sheetId="6" r:id="rId6"/>
     <sheet name="Incubator box" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="516">
   <si>
     <t>Parts List</t>
   </si>
@@ -1576,12 +1575,21 @@
   </si>
   <si>
     <t>DMSP900R</t>
+  </si>
+  <si>
+    <t>Small Positive lens</t>
+  </si>
+  <si>
+    <t>AC254-100-A</t>
+  </si>
+  <si>
+    <t>f = 100 mm, Ø1" Achromatic Doublet, ARC: 400 - 700 nm </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
@@ -2031,7 +2039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -3531,11 +3539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3708,7 +3716,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -3945,7 +3953,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -4078,304 +4086,307 @@
         <v>152</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="14"/>
+    </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>513</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="D32" s="6">
-        <v>122.55</v>
+        <v>5.95</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" ref="F32:F38" si="2">D32*E32</f>
-        <v>122.55</v>
+        <f t="shared" ref="F32" si="2">D32*E32</f>
+        <v>5.95</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="D33" s="6">
-        <v>67.16</v>
+        <v>39.770000000000003</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" s="6">
-        <f t="shared" si="2"/>
-        <v>67.16</v>
+        <f t="shared" ref="F33:F37" si="3">D33*E33</f>
+        <v>39.770000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D34" s="6">
-        <v>5.95</v>
+        <v>9.18</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" si="2"/>
-        <v>5.95</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D35" s="6">
-        <v>4.01</v>
+        <v>7.96</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="6">
-        <f t="shared" si="2"/>
-        <v>4.01</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D36" s="6">
-        <v>9.18</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>152</v>
+        <f t="shared" si="3"/>
+        <v>4.1900000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D37" s="6">
-        <v>7.96</v>
+        <v>22.73</v>
       </c>
       <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <f t="shared" si="3"/>
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="D38" s="6">
+        <v>3.86</v>
+      </c>
+      <c r="E38" s="19">
         <v>0</v>
       </c>
-      <c r="F37" s="6">
-        <f t="shared" si="2"/>
+      <c r="F38" s="14">
+        <f>D38*E38</f>
         <v>0</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" t="s">
-        <v>140</v>
-      </c>
-      <c r="D38" s="6">
-        <v>22.73</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" s="6">
-        <f t="shared" si="2"/>
-        <v>22.73</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
-        <v>495</v>
+        <v>515</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="19" t="s">
-        <v>494</v>
+      <c r="C39" t="s">
+        <v>514</v>
       </c>
       <c r="D39" s="6">
-        <v>3.86</v>
+        <v>60.87</v>
       </c>
       <c r="E39" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="14">
         <f>D39*E39</f>
-        <v>0</v>
-      </c>
-      <c r="G39" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="3"/>
-      <c r="F40" s="6"/>
+        <v>60.87</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D42" s="6">
-        <v>81.97</v>
+        <v>122.55</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" s="6">
-        <f t="shared" ref="F42:F48" si="3">D42*E42</f>
-        <v>81.97</v>
+        <f t="shared" ref="F42:F48" si="4">D42*E42</f>
+        <v>122.55</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="D43" s="6">
-        <v>5.95</v>
+        <v>67.16</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43" s="6">
-        <f t="shared" si="3"/>
-        <v>5.95</v>
+        <f t="shared" si="4"/>
+        <v>67.16</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="D44" s="6">
-        <v>4.01</v>
+        <v>5.95</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" s="6">
-        <f t="shared" si="3"/>
-        <v>4.01</v>
+        <f t="shared" si="4"/>
+        <v>5.95</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="D45" s="6">
-        <v>9.18</v>
+        <v>4.01</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G45" t="s">
-        <v>152</v>
+        <f t="shared" si="4"/>
+        <v>4.01</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D46" s="6">
-        <v>7.96</v>
+        <v>9.18</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G46" t="s">
@@ -4384,47 +4395,50 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D47" s="6">
-        <v>22.73</v>
+        <v>7.96</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="6">
-        <f t="shared" si="3"/>
-        <v>22.73</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="D48" s="6">
-        <v>117.41</v>
+        <v>22.73</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" s="6">
-        <f t="shared" si="3"/>
-        <v>117.41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="4"/>
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
         <v>495</v>
       </c>
@@ -4438,68 +4452,256 @@
         <v>3.86</v>
       </c>
       <c r="E49" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="14">
         <f>D49*E49</f>
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="3"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="6">
+        <v>81.97</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="6">
+        <f t="shared" ref="F52:F58" si="5">D52*E52</f>
+        <v>81.97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="6">
+        <v>5.95</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="6">
+        <f t="shared" si="5"/>
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="6">
+        <v>4.01</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="6">
+        <f t="shared" si="5"/>
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="6">
+        <v>9.18</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="6">
+        <v>7.96</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" s="6">
+        <v>22.73</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="6">
+        <f t="shared" si="5"/>
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D58" s="6">
+        <v>117.41</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="6">
+        <f t="shared" si="5"/>
+        <v>117.41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="D59" s="6">
         <v>3.86</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
+      <c r="E59" s="19">
+        <v>1</v>
+      </c>
+      <c r="F59" s="14">
+        <f>D59*E59</f>
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D62" s="6">
         <v>79.569999999999993</v>
       </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="6">
-        <f>D52*E52</f>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="6">
+        <f>D62*E62</f>
         <v>79.569999999999993</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
-      <c r="D53" s="6"/>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="3"/>
+      <c r="D63" s="6"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="F55" s="6">
-        <f>SUM(F3:F52)</f>
-        <v>1907.8800000000003</v>
+      <c r="F65" s="6">
+        <f>SUM(F3:F62)</f>
+        <v>2041.3900000000003</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7192,7 +7394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
@@ -7927,7 +8129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8178,7 +8380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8607,7 +8809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Changed FS Rocker Switch
</commit_message>
<xml_diff>
--- a/LifeHack-Parts.xlsx
+++ b/LifeHack-Parts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\LifeHack\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FA3807-CDF5-46FA-8F2A-22B066EE125E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2"/>
+    <workbookView xWindow="-28920" yWindow="2505" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Excitation Module" sheetId="2" r:id="rId1"/>
@@ -1013,12 +1014,6 @@
     <t>735-0747</t>
   </si>
   <si>
-    <t>Rocker switch</t>
-  </si>
-  <si>
-    <t>533-2964</t>
-  </si>
-  <si>
     <t>Arduino enclosure</t>
   </si>
   <si>
@@ -1593,12 +1588,18 @@
   </si>
   <si>
     <t>Includes: Objective basket if requested through Cairn research</t>
+  </si>
+  <si>
+    <t>907-7071</t>
+  </si>
+  <si>
+    <t>DPDT Rocker switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
@@ -2049,7 +2050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2876,7 +2877,7 @@
         <v>157</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>11</v>
@@ -2894,10 +2895,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>11</v>
@@ -2915,7 +2916,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>238</v>
@@ -2936,10 +2937,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>11</v>
@@ -2957,10 +2958,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>11</v>
@@ -3200,7 +3201,7 @@
         <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -3221,7 +3222,7 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -3549,7 +3550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3852,13 +3853,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D17" s="6">
         <v>19.309999999999999</v>
@@ -4074,13 +4075,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D29" s="6">
         <v>3.86</v>
@@ -4105,7 +4106,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="6"/>
@@ -4246,13 +4247,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D38" s="6">
         <v>3.86</v>
@@ -4270,13 +4271,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D39" s="6">
         <v>60.87</v>
@@ -4450,13 +4451,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D49" s="6">
         <v>3.86</v>
@@ -4637,13 +4638,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="18" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D59" s="6">
         <v>3.86</v>
@@ -4707,11 +4708,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4788,7 +4789,7 @@
         <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -4809,7 +4810,7 @@
         <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4830,7 +4831,7 @@
         <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4851,7 +4852,7 @@
         <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -4872,7 +4873,7 @@
         <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -4885,7 +4886,7 @@
         <v>3015.27</v>
       </c>
       <c r="G9" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -4907,7 +4908,7 @@
         <v>186</v>
       </c>
       <c r="C12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -4929,7 +4930,7 @@
         <v>188</v>
       </c>
       <c r="C13" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -4942,18 +4943,18 @@
         <v>18047.43</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -4966,7 +4967,7 @@
         <v>2250</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H14" s="10"/>
     </row>
@@ -4978,7 +4979,7 @@
         <v>190</v>
       </c>
       <c r="C15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -5262,7 +5263,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -5769,7 +5770,7 @@
         <v>214</v>
       </c>
       <c r="B63" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -5791,7 +5792,7 @@
         <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
@@ -6137,7 +6138,7 @@
         <v>120</v>
       </c>
       <c r="G82" s="18" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -6189,7 +6190,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E86" s="10"/>
       <c r="F86" s="10"/>
@@ -6199,10 +6200,10 @@
         <v>291</v>
       </c>
       <c r="B87" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C87" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -6526,10 +6527,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B106" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C106" t="s">
         <v>311</v>
@@ -6639,10 +6640,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B112" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C112" t="s">
         <v>311</v>
@@ -6660,13 +6661,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>422</v>
+      </c>
+      <c r="B113" t="s">
+        <v>423</v>
+      </c>
+      <c r="C113" t="s">
         <v>424</v>
-      </c>
-      <c r="B113" t="s">
-        <v>425</v>
-      </c>
-      <c r="C113" t="s">
-        <v>426</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -6681,10 +6682,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>325</v>
+        <v>518</v>
       </c>
       <c r="B114" t="s">
-        <v>326</v>
+        <v>517</v>
       </c>
       <c r="C114" t="s">
         <v>311</v>
@@ -6693,16 +6694,16 @@
         <v>1</v>
       </c>
       <c r="E114" s="10">
-        <v>5.25</v>
+        <v>7.6</v>
       </c>
       <c r="F114" s="10">
         <f t="shared" si="2"/>
-        <v>5.25</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B115" t="s">
         <v>93</v>
@@ -6724,10 +6725,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B116" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C116" t="s">
         <v>311</v>
@@ -6745,10 +6746,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B117" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C117" t="s">
         <v>311</v>
@@ -6766,10 +6767,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B118" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C118" t="s">
         <v>311</v>
@@ -6787,10 +6788,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B119" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C119" t="s">
         <v>311</v>
@@ -6808,10 +6809,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B120" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C120" t="s">
         <v>311</v>
@@ -6830,10 +6831,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B121" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C121" t="s">
         <v>311</v>
@@ -6852,10 +6853,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B122" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C122" t="s">
         <v>311</v>
@@ -6878,27 +6879,27 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E124" s="10"/>
       <c r="F124" s="10"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E125" s="10"/>
       <c r="F125" s="10"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B126" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C126" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D126">
         <v>1</v>
@@ -6914,10 +6915,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B127" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C127" t="s">
         <v>11</v>
@@ -6935,7 +6936,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B128" s="21" t="s">
         <v>296</v>
@@ -6956,7 +6957,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B129" t="s">
         <v>130</v>
@@ -6980,7 +6981,7 @@
         <v>256</v>
       </c>
       <c r="B130" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C130" t="s">
         <v>11</v>
@@ -6998,10 +6999,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B131" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C131" t="s">
         <v>11</v>
@@ -7041,10 +7042,10 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B133" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C133" t="s">
         <v>11</v>
@@ -7062,7 +7063,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B134" t="s">
         <v>93</v>
@@ -7087,20 +7088,20 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B137" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C137" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -7116,13 +7117,13 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B138" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C138" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -7138,13 +7139,13 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B139" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C139" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -7164,17 +7165,17 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E141" s="10"/>
       <c r="F141" s="10"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B142" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C142" t="s">
         <v>57</v>
@@ -7193,10 +7194,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B143" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C143" t="s">
         <v>57</v>
@@ -7215,10 +7216,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B144" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C144" t="s">
         <v>57</v>
@@ -7237,10 +7238,10 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B145" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C145" t="s">
         <v>57</v>
@@ -7259,10 +7260,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B146" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C146" t="s">
         <v>57</v>
@@ -7281,10 +7282,10 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B147" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C147" t="s">
         <v>57</v>
@@ -7303,10 +7304,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B148" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C148" t="s">
         <v>57</v>
@@ -7325,10 +7326,10 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B149" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C149" t="s">
         <v>57</v>
@@ -7347,10 +7348,10 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B150" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C150" t="s">
         <v>57</v>
@@ -7369,10 +7370,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B151" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C151" t="s">
         <v>11</v>
@@ -7390,10 +7391,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B152" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C152" t="s">
         <v>11</v>
@@ -7415,7 +7416,7 @@
       </c>
       <c r="F154" s="10">
         <f>SUM(F2:F152)</f>
-        <v>80315.787000000011</v>
+        <v>80318.137000000017</v>
       </c>
     </row>
   </sheetData>
@@ -7425,11 +7426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7442,7 +7443,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -7475,10 +7476,10 @@
         <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -7802,10 +7803,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C22" t="s">
         <v>311</v>
@@ -7912,10 +7913,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B28" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C28" t="s">
         <v>311</v>
@@ -7933,13 +7934,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>422</v>
+      </c>
+      <c r="B29" t="s">
+        <v>423</v>
+      </c>
+      <c r="C29" t="s">
         <v>424</v>
-      </c>
-      <c r="B29" t="s">
-        <v>425</v>
-      </c>
-      <c r="C29" t="s">
-        <v>426</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -7954,10 +7955,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>518</v>
       </c>
       <c r="B30" t="s">
-        <v>326</v>
+        <v>517</v>
       </c>
       <c r="C30" t="s">
         <v>311</v>
@@ -7966,16 +7967,16 @@
         <v>1</v>
       </c>
       <c r="E30" s="10">
-        <v>5.25</v>
+        <v>7.6</v>
       </c>
       <c r="F30" s="10">
         <f t="shared" si="0"/>
-        <v>5.25</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B31" t="s">
         <v>93</v>
@@ -7997,10 +7998,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B32" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C32" t="s">
         <v>311</v>
@@ -8018,10 +8019,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B33" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C33" t="s">
         <v>311</v>
@@ -8039,10 +8040,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B34" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C34" t="s">
         <v>311</v>
@@ -8060,10 +8061,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B35" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C35" t="s">
         <v>311</v>
@@ -8081,10 +8082,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B36" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C36" t="s">
         <v>311</v>
@@ -8103,10 +8104,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B37" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C37" t="s">
         <v>311</v>
@@ -8125,10 +8126,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B38" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C38" t="s">
         <v>311</v>
@@ -8151,7 +8152,7 @@
       </c>
       <c r="F41" s="10">
         <f>SUM(F3:F38)</f>
-        <v>7725.7400000000052</v>
+        <v>7728.0900000000056</v>
       </c>
     </row>
   </sheetData>
@@ -8160,7 +8161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8177,7 +8178,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -8207,13 +8208,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -8229,10 +8230,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -8250,7 +8251,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>296</v>
@@ -8271,7 +8272,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B6" t="s">
         <v>130</v>
@@ -8295,7 +8296,7 @@
         <v>256</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -8313,10 +8314,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -8356,10 +8357,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -8377,7 +8378,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B11" t="s">
         <v>93</v>
@@ -8411,7 +8412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8451,20 +8452,20 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s">
         <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -8479,10 +8480,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C5" t="s">
         <v>311</v>
@@ -8501,10 +8502,10 @@
     </row>
     <row r="6" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>311</v>
@@ -8522,10 +8523,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>311</v>
@@ -8543,10 +8544,10 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>311</v>
@@ -8564,13 +8565,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>383</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>384</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>385</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -8585,10 +8586,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>311</v>
@@ -8613,17 +8614,17 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -8641,10 +8642,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -8662,10 +8663,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -8683,10 +8684,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B16" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -8710,7 +8711,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="14"/>
@@ -8718,13 +8719,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>396</v>
+      </c>
+      <c r="B19" t="s">
+        <v>397</v>
+      </c>
+      <c r="C19" t="s">
         <v>398</v>
-      </c>
-      <c r="B19" t="s">
-        <v>399</v>
-      </c>
-      <c r="C19" t="s">
-        <v>400</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -8739,13 +8740,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B20" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C20" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -8760,13 +8761,13 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B21" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C21" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -8786,14 +8787,14 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -8840,7 +8841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8877,14 +8878,14 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D2" s="10"/>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B3" t="s">
         <v>93</v>
@@ -8909,14 +8910,14 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D5" s="10"/>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B6" t="s">
         <v>93</v>
@@ -8934,7 +8935,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B7" t="s">
         <v>93</v>
@@ -8952,7 +8953,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B8" t="s">
         <v>93</v>
@@ -8969,7 +8970,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B9" t="s">
         <v>93</v>
@@ -8986,7 +8987,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B10" t="s">
         <v>93</v>
@@ -9003,7 +9004,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B11" t="s">
         <v>93</v>
@@ -9020,7 +9021,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B12" t="s">
         <v>93</v>
@@ -9037,7 +9038,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B13" t="s">
         <v>93</v>
@@ -9054,7 +9055,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B14" t="s">
         <v>93</v>
@@ -9071,7 +9072,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B15" t="s">
         <v>93</v>
@@ -9088,7 +9089,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B16" t="s">
         <v>93</v>
@@ -9105,7 +9106,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B17" t="s">
         <v>93</v>
@@ -9122,7 +9123,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B18" t="s">
         <v>93</v>
@@ -9139,7 +9140,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B19" t="s">
         <v>93</v>
@@ -9156,13 +9157,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B20" t="s">
         <v>311</v>
       </c>
       <c r="C20" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D20" s="10">
         <v>19.3</v>
@@ -9177,12 +9178,12 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B23" t="s">
         <v>93</v>
@@ -9199,7 +9200,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B24" t="s">
         <v>93</v>
@@ -9216,7 +9217,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B25" t="s">
         <v>93</v>
@@ -9233,7 +9234,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B26" t="s">
         <v>93</v>
@@ -9250,7 +9251,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B27" t="s">
         <v>93</v>
@@ -9267,7 +9268,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B28" t="s">
         <v>93</v>
@@ -9284,7 +9285,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B29" t="s">
         <v>93</v>
@@ -9301,7 +9302,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B30" t="s">
         <v>93</v>
@@ -9318,13 +9319,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B31" t="s">
         <v>311</v>
       </c>
       <c r="C31" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D31" s="10">
         <v>19.3</v>
@@ -9339,12 +9340,12 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B34" t="s">
         <v>93</v>
@@ -9361,7 +9362,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B35" t="s">
         <v>93</v>
@@ -9378,7 +9379,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B36" t="s">
         <v>93</v>
@@ -9395,7 +9396,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B37" t="s">
         <v>93</v>
@@ -9412,7 +9413,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B38" t="s">
         <v>93</v>
@@ -9429,7 +9430,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B39" t="s">
         <v>93</v>
@@ -9447,7 +9448,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B40" t="s">
         <v>93</v>
@@ -9464,13 +9465,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B41" t="s">
         <v>311</v>
       </c>
       <c r="C41" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D41" s="10">
         <v>19.3</v>
@@ -9485,14 +9486,14 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D43" s="10"/>
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B44" t="s">
         <v>93</v>
@@ -9510,7 +9511,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B45" t="s">
         <v>93</v>
@@ -9528,7 +9529,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B46" t="s">
         <v>93</v>
@@ -9546,7 +9547,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B47" t="s">
         <v>93</v>
@@ -9564,7 +9565,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B48" t="s">
         <v>93</v>
@@ -9582,12 +9583,12 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B51" t="s">
         <v>93</v>
@@ -9604,7 +9605,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B52" t="s">
         <v>93</v>
@@ -9621,7 +9622,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B53" t="s">
         <v>93</v>
@@ -9638,7 +9639,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B54" t="s">
         <v>93</v>
@@ -9656,7 +9657,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B55" t="s">
         <v>93</v>
@@ -9678,20 +9679,20 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D57" s="10"/>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B58" t="s">
         <v>311</v>
       </c>
       <c r="C58" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D58" s="10">
         <v>10.66</v>
@@ -9706,13 +9707,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B59" t="s">
         <v>311</v>
       </c>
       <c r="C59" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D59" s="10">
         <v>2.38</v>
@@ -9727,13 +9728,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B60" t="s">
         <v>311</v>
       </c>
       <c r="C60" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D60" s="10">
         <v>13.98</v>
@@ -9748,7 +9749,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D61" s="10"/>
       <c r="F61" s="10"/>
@@ -9756,7 +9757,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D62" s="10"/>
       <c r="F62" s="10"/>
@@ -9768,17 +9769,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D64" s="10"/>
       <c r="F64" s="10"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B65" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C65">
         <v>14130</v>
@@ -9796,10 +9797,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B66" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C66">
         <v>10035</v>
@@ -9817,10 +9818,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B67" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C67">
         <v>10034</v>
@@ -9838,10 +9839,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B68" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C68">
         <v>90051</v>
@@ -9859,10 +9860,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B69" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C69" t="s">
         <v>93</v>

</xml_diff>